<commit_message>
expose SheetCell name bug with unicode chars
</commit_message>
<xml_diff>
--- a/data/book_1904_ptbr.xlsx
+++ b/data/book_1904_ptbr.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10513"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/.julia/dev/XLSX/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4F7B59-CA0C-DE42-AD4E-D2DC4D22A1FF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="90" windowWidth="9420" windowHeight="6300"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="NEGOCIAÇÕES Descrição" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="101716"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Coluna A</t>
   </si>
@@ -64,12 +71,15 @@
   </si>
   <si>
     <t>D3</t>
+  </si>
+  <si>
+    <t>Negociações</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -118,14 +128,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -163,9 +176,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -198,9 +211,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,9 +263,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -408,19 +455,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>10</v>
       </c>
@@ -448,7 +495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>20</v>
       </c>
@@ -462,7 +509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>30</v>
       </c>
@@ -484,16 +531,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -501,7 +548,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -515,7 +562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -541,15 +588,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.49212598499999999" footer="0.49212598499999999"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D37CE1-455F-FD45-BA8F-4EF5FD990572}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>